<commit_message>
adds preguntas y graficas
</commit_message>
<xml_diff>
--- a/Graficas.xlsx
+++ b/Graficas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/katherinegarcia/Documents/Semestre7/SisOps/EjerciciosP2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B03F342-D115-9A44-B9FA-A611A8DEEF0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EB2B4C6-007E-5B4A-8384-C8209C08177C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="4" xr2:uid="{842B33A2-C5BF-E74C-A756-B85769930930}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="5" xr2:uid="{842B33A2-C5BF-E74C-A756-B85769930930}"/>
   </bookViews>
   <sheets>
     <sheet name="G1" sheetId="1" r:id="rId1"/>
@@ -18,22 +18,9 @@
     <sheet name="G3" sheetId="3" r:id="rId3"/>
     <sheet name="G4" sheetId="4" r:id="rId4"/>
     <sheet name="TODAS" sheetId="5" r:id="rId5"/>
+    <sheet name="Preguntas" sheetId="6" r:id="rId6"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">'G4'!$B$18:$G$18</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">'G4'!$B$5:$G$6</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">'G4'!$B$18:$G$18</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">'G4'!$B$5:$G$6</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">'G4'!$B$18:$G$18</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">'G4'!$B$5:$G$6</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">'G4'!$B$18:$G$18</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">'G4'!$B$5:$G$6</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">'G4'!$B$18:$G$18</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">'G4'!$B$5:$G$6</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">'G4'!$B$18:$G$18</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">'G4'!$B$5:$G$6</definedName>
-  </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -53,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="28">
   <si>
     <t>2 THREADS</t>
   </si>
@@ -110,6 +97,33 @@
   </si>
   <si>
     <t>PROM SECUENCIAL</t>
+  </si>
+  <si>
+    <t>1. ¿Cuál es el modelo de paralelismo más rápido en los 6 escenarios?</t>
+  </si>
+  <si>
+    <t>Los modelos de paralelización mas rápidos son:</t>
+  </si>
+  <si>
+    <t>Archivos</t>
+  </si>
+  <si>
+    <t>Funciones</t>
+  </si>
+  <si>
+    <t>2. ¿Cuál opción modelo de paralelismo tomaría usted y por qué?</t>
+  </si>
+  <si>
+    <t>Depende de los recursos que tengamos y objetivo que el proyecto tenga. En este caso, el modelo más consistente fue la paralelización por archivos. A pesar de las restricciones que se tenían.</t>
+  </si>
+  <si>
+    <t>3. ¿Recomendaría paralelizar tanto archivos y funciones al mismo tiempo?</t>
+  </si>
+  <si>
+    <t>En este caso, el modelo de paralelizacion por funciones y archivos, es el caso mas tardado. Por lo que no lo recomendariamos debido a la limitacion de recursos que se posee.</t>
+  </si>
+  <si>
+    <t>4. Cuál es el factor de mejora de pasar de 1 Core a 2 Core para el proceso que paraleliza los archivos</t>
   </si>
 </sst>
 </file>
@@ -255,7 +269,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -263,9 +277,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -282,6 +293,13 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1362,6 +1380,665 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>PROMEDIO TOTAL DE CADA ESCENARIO</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-GT"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>TODAS!$B$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>PROM ARCHIVOS  </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>TODAS!$C$2:$H$3</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="6"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>1 THREAD</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>4 THREADS</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>2 THREADS</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>4 THREADS</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>8 THREADS</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>8 THREADS</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>1 CORE</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>2 CORES</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>4 CORES</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>TODAS!$C$5:$H$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>9.683720000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>50.752469999999995</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16.769690000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20.26613</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>18.319382000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>19.639316999999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-9B5F-0B4E-9E52-4F27AE6DCB21}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>TODAS!$B$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>PROM FUNCIONES</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>TODAS!$C$2:$H$3</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="6"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>1 THREAD</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>4 THREADS</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>2 THREADS</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>4 THREADS</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>8 THREADS</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>8 THREADS</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>1 CORE</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>2 CORES</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>4 CORES</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>TODAS!$C$6:$H$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>42.643739999999994</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>30.639780000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>26.576080000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30.234349999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>29.809720000000006</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>13.24981</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-9B5F-0B4E-9E52-4F27AE6DCB21}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>TODAS!$B$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>PROM ARCHIVOS Y FUNCIONES</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>TODAS!$C$2:$H$3</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="6"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>1 THREAD</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>4 THREADS</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>2 THREADS</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>4 THREADS</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>8 THREADS</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>8 THREADS</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>1 CORE</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>2 CORES</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>4 CORES</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>TODAS!$C$7:$H$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>42.149899999999995</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>56.745457999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>24.642440000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>28.830159999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>38.51455</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>18.867979999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-9B5F-0B4E-9E52-4F27AE6DCB21}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="527127744"/>
+        <c:axId val="527129392"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="527127744"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-GT"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-GT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="527129392"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="527129392"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>PROMEDIO EN SEGUNDOS</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-GT"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-GT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="527127744"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-GT"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-GT"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
@@ -4086,6 +4763,46 @@
 </file>
 
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors10.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -4961,7 +5678,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style10.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -5477,7 +6194,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -5993,7 +6710,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -6509,7 +7226,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -7025,7 +7742,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -7541,7 +8258,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -8057,7 +8774,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -8573,7 +9290,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style8.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -9089,20 +9806,536 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style9.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>194734</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>84667</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>728846</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>37189</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>601133</xdr:colOff>
-      <xdr:row>45</xdr:row>
-      <xdr:rowOff>84666</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>462898</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>154298</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -9130,15 +10363,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>186267</xdr:colOff>
+      <xdr:colOff>245613</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>33866</xdr:rowOff>
+      <xdr:rowOff>21997</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>609600</xdr:colOff>
+      <xdr:colOff>668946</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>135466</xdr:rowOff>
+      <xdr:rowOff>123597</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -9170,16 +10403,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>96520</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>5080</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>675640</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>553720</xdr:colOff>
-      <xdr:row>46</xdr:row>
-      <xdr:rowOff>106680</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>309880</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>116840</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -9247,16 +10480,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>96520</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>5080</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>655320</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>553720</xdr:colOff>
-      <xdr:row>46</xdr:row>
-      <xdr:rowOff>106680</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>289560</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>116840</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -9328,15 +10561,15 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>96520</xdr:colOff>
-      <xdr:row>33</xdr:row>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>716280</xdr:colOff>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>5080</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>553720</xdr:colOff>
-      <xdr:row>46</xdr:row>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>350520</xdr:colOff>
+      <xdr:row>32</xdr:row>
       <xdr:rowOff>106680</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -9404,16 +10637,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>477520</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>60960</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>111760</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>162560</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -9468,6 +10701,49 @@
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>50800</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2BAC841C-25B5-3941-BE83-8CF8F850A4DF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -9784,7 +11060,7 @@
   <dimension ref="A2:G18"/>
   <sheetViews>
     <sheetView zoomScale="107" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18:G18"/>
+      <selection activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9796,246 +11072,246 @@
       <c r="B2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="10"/>
+      <c r="F3" s="9"/>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5" t="s">
+      <c r="C5" s="12"/>
+      <c r="D5" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="6" t="s">
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="5" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="E6" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="F6" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="G6" s="6" t="s">
+      <c r="G6" s="5" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B7" s="7">
+      <c r="B7" s="6">
         <v>9.4786999999999999</v>
       </c>
-      <c r="C7" s="7">
+      <c r="C7" s="6">
         <v>9.7462999999999997</v>
       </c>
-      <c r="D7" s="7">
+      <c r="D7" s="6">
         <v>9.4983000000000004</v>
       </c>
-      <c r="E7" s="7">
+      <c r="E7" s="6">
         <v>10.218299999999999</v>
       </c>
-      <c r="F7" s="7">
+      <c r="F7" s="6">
         <v>10.097300000000001</v>
       </c>
-      <c r="G7" s="8">
+      <c r="G7" s="7">
         <v>9.0515000000000008</v>
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B8" s="9">
+      <c r="B8" s="8">
         <v>9.2720000000000002</v>
       </c>
-      <c r="C8" s="9">
+      <c r="C8" s="8">
         <v>9.5748999999999995</v>
       </c>
-      <c r="D8" s="9">
+      <c r="D8" s="8">
         <v>9.7133000000000003</v>
       </c>
-      <c r="E8" s="9">
+      <c r="E8" s="8">
         <v>9.7383000000000006</v>
       </c>
-      <c r="F8" s="9">
+      <c r="F8" s="8">
         <v>10.2369</v>
       </c>
-      <c r="G8" s="9">
+      <c r="G8" s="8">
         <v>10.3802</v>
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B9" s="9">
+      <c r="B9" s="8">
         <v>9.6378000000000004</v>
       </c>
-      <c r="C9" s="9">
+      <c r="C9" s="8">
         <v>9.5414999999999992</v>
       </c>
-      <c r="D9" s="9">
+      <c r="D9" s="8">
         <v>9.5815999999999999</v>
       </c>
-      <c r="E9" s="9">
+      <c r="E9" s="8">
         <v>9.5239999999999991</v>
       </c>
-      <c r="F9" s="9">
+      <c r="F9" s="8">
         <v>10.4696</v>
       </c>
-      <c r="G9" s="9">
+      <c r="G9" s="8">
         <v>9.7089999999999996</v>
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B10" s="9">
+      <c r="B10" s="8">
         <v>9.6868999999999996</v>
       </c>
-      <c r="C10" s="9">
+      <c r="C10" s="8">
         <v>9.5985999999999994</v>
       </c>
-      <c r="D10" s="9">
+      <c r="D10" s="8">
         <v>9.6021999999999998</v>
       </c>
-      <c r="E10" s="9">
+      <c r="E10" s="8">
         <v>9.8321000000000005</v>
       </c>
-      <c r="F10" s="9">
+      <c r="F10" s="8">
         <v>10.0007</v>
       </c>
-      <c r="G10" s="9">
+      <c r="G10" s="8">
         <v>9.5370000000000008</v>
       </c>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B11" s="9">
+      <c r="B11" s="8">
         <v>9.5414999999999992</v>
       </c>
-      <c r="C11" s="9">
+      <c r="C11" s="8">
         <v>9.6329999999999991</v>
       </c>
-      <c r="D11" s="9">
+      <c r="D11" s="8">
         <v>9.9804999999999993</v>
       </c>
-      <c r="E11" s="9">
+      <c r="E11" s="8">
         <v>10.010999999999999</v>
       </c>
-      <c r="F11" s="9">
+      <c r="F11" s="8">
         <v>10.040100000000001</v>
       </c>
-      <c r="G11" s="9">
+      <c r="G11" s="8">
         <v>9.4489000000000001</v>
       </c>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B12" s="9">
+      <c r="B12" s="8">
         <v>9.6655999999999995</v>
       </c>
-      <c r="C12" s="9">
+      <c r="C12" s="8">
         <v>9.3369</v>
       </c>
-      <c r="D12" s="9">
+      <c r="D12" s="8">
         <v>9.7888000000000002</v>
       </c>
-      <c r="E12" s="9">
+      <c r="E12" s="8">
         <v>10.4528</v>
       </c>
-      <c r="F12" s="9">
+      <c r="F12" s="8">
         <v>9.9976000000000003</v>
       </c>
-      <c r="G12" s="9">
+      <c r="G12" s="8">
         <v>9.3358000000000008</v>
       </c>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B13" s="9">
+      <c r="B13" s="8">
         <v>9.9542999999999999</v>
       </c>
-      <c r="C13" s="9">
+      <c r="C13" s="8">
         <v>9.6662999999999997</v>
       </c>
-      <c r="D13" s="9">
+      <c r="D13" s="8">
         <v>9.6885999999999992</v>
       </c>
-      <c r="E13" s="9">
+      <c r="E13" s="8">
         <v>10.301299999999999</v>
       </c>
-      <c r="F13" s="9">
+      <c r="F13" s="8">
         <v>10.3345</v>
       </c>
-      <c r="G13" s="9">
+      <c r="G13" s="8">
         <v>9.2667000000000002</v>
       </c>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B14" s="9">
+      <c r="B14" s="8">
         <v>9.6857000000000006</v>
       </c>
-      <c r="C14" s="9">
+      <c r="C14" s="8">
         <v>9.8353000000000002</v>
       </c>
-      <c r="D14" s="9">
+      <c r="D14" s="8">
         <v>10.270099999999999</v>
       </c>
-      <c r="E14" s="9">
+      <c r="E14" s="8">
         <v>9.9514999999999993</v>
       </c>
-      <c r="F14" s="9">
+      <c r="F14" s="8">
         <v>10.2178</v>
       </c>
-      <c r="G14" s="9">
+      <c r="G14" s="8">
         <v>9.8495000000000008</v>
       </c>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B15" s="9">
+      <c r="B15" s="8">
         <v>9.9345599999999994</v>
       </c>
-      <c r="C15" s="9">
+      <c r="C15" s="8">
         <v>9.6545000000000005</v>
       </c>
-      <c r="D15" s="9">
+      <c r="D15" s="8">
         <v>10.023899999999999</v>
       </c>
-      <c r="E15" s="9">
+      <c r="E15" s="8">
         <v>10.2143</v>
       </c>
-      <c r="F15" s="9">
+      <c r="F15" s="8">
         <v>10.3223</v>
       </c>
-      <c r="G15" s="9">
+      <c r="G15" s="8">
         <v>9.5356000000000005</v>
       </c>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B16" s="9">
+      <c r="B16" s="8">
         <v>9.8536999999999999</v>
       </c>
-      <c r="C16" s="9">
+      <c r="C16" s="8">
         <v>9.5647000000000002</v>
       </c>
-      <c r="D16" s="9">
+      <c r="D16" s="8">
         <v>9.8438999999999997</v>
       </c>
-      <c r="E16" s="9">
+      <c r="E16" s="8">
         <v>10.177</v>
       </c>
-      <c r="F16" s="9">
+      <c r="F16" s="8">
         <v>10.409800000000001</v>
       </c>
-      <c r="G16" s="9">
+      <c r="G16" s="8">
         <v>9.3801000000000005</v>
       </c>
     </row>
@@ -10113,7 +11389,7 @@
   <dimension ref="A2:G18"/>
   <sheetViews>
     <sheetView zoomScale="125" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:G6"/>
+      <selection activeCell="K34" sqref="K34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10129,36 +11405,36 @@
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5" t="s">
+      <c r="C5" s="12"/>
+      <c r="D5" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="6" t="s">
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="5" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="E6" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="F6" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="G6" s="6" t="s">
+      <c r="G6" s="5" t="s">
         <v>3</v>
       </c>
     </row>
@@ -10435,7 +11711,7 @@
   <dimension ref="A2:G18"/>
   <sheetViews>
     <sheetView zoomScale="125" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18:G18"/>
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10451,36 +11727,36 @@
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5" t="s">
+      <c r="C5" s="12"/>
+      <c r="D5" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="6" t="s">
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="5" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="E6" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="F6" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="G6" s="6" t="s">
+      <c r="G6" s="5" t="s">
         <v>3</v>
       </c>
     </row>
@@ -10757,7 +12033,7 @@
   <dimension ref="A2:G18"/>
   <sheetViews>
     <sheetView zoomScale="125" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18:G18"/>
+      <selection activeCell="I44" sqref="I44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10773,36 +12049,36 @@
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5" t="s">
+      <c r="C5" s="12"/>
+      <c r="D5" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="6" t="s">
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="5" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="E6" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="F6" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="G6" s="6" t="s">
+      <c r="G6" s="5" t="s">
         <v>3</v>
       </c>
     </row>
@@ -10810,7 +12086,7 @@
       <c r="B7" s="2">
         <v>45.866599999999998</v>
       </c>
-      <c r="C7" s="11">
+      <c r="C7" s="10">
         <v>55.872799999999998</v>
       </c>
       <c r="D7" s="2">
@@ -10830,7 +12106,7 @@
       <c r="B8" s="2">
         <v>45.418199999999999</v>
       </c>
-      <c r="C8" s="12">
+      <c r="C8" s="11">
         <v>56.011899999999997</v>
       </c>
       <c r="D8" s="2">
@@ -10850,7 +12126,7 @@
       <c r="B9" s="2">
         <v>46.027799999999999</v>
       </c>
-      <c r="C9" s="12">
+      <c r="C9" s="11">
         <v>55.803800000000003</v>
       </c>
       <c r="D9" s="2">
@@ -10870,7 +12146,7 @@
       <c r="B10" s="2">
         <v>45.982900000000001</v>
       </c>
-      <c r="C10" s="12">
+      <c r="C10" s="11">
         <v>60.037280000000003</v>
       </c>
       <c r="D10" s="2">
@@ -10890,7 +12166,7 @@
       <c r="B11" s="2">
         <v>47.0197</v>
       </c>
-      <c r="C11" s="12">
+      <c r="C11" s="11">
         <v>55.130299999999998</v>
       </c>
       <c r="D11" s="2">
@@ -10910,7 +12186,7 @@
       <c r="B12" s="2">
         <v>46.637900000000002</v>
       </c>
-      <c r="C12" s="12">
+      <c r="C12" s="11">
         <v>57.357599999999998</v>
       </c>
       <c r="D12" s="2">
@@ -10930,7 +12206,7 @@
       <c r="B13" s="2">
         <v>46.197400000000002</v>
       </c>
-      <c r="C13" s="12">
+      <c r="C13" s="11">
         <v>57.073599999999999</v>
       </c>
       <c r="D13" s="2">
@@ -10950,7 +12226,7 @@
       <c r="B14" s="2">
         <v>45.838900000000002</v>
       </c>
-      <c r="C14" s="12">
+      <c r="C14" s="11">
         <v>57.116700000000002</v>
       </c>
       <c r="D14" s="2">
@@ -10970,7 +12246,7 @@
       <c r="B15" s="2">
         <v>6.0119999999999996</v>
       </c>
-      <c r="C15" s="12">
+      <c r="C15" s="11">
         <v>57.490299999999998</v>
       </c>
       <c r="D15" s="2">
@@ -10990,7 +12266,7 @@
       <c r="B16" s="2">
         <v>46.497599999999998</v>
       </c>
-      <c r="C16" s="12">
+      <c r="C16" s="11">
         <v>55.560299999999998</v>
       </c>
       <c r="D16" s="2">
@@ -11078,43 +12354,43 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FC59D95-BFDA-464E-9EC5-045460106246}">
   <dimension ref="B2:H7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I39" sqref="I39:I40"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="2" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5" t="s">
+      <c r="D2" s="12"/>
+      <c r="E2" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="6" t="s">
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="5" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="H3" s="5" t="s">
         <v>3</v>
       </c>
     </row>
@@ -11218,4 +12494,171 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93C50910-1F7A-B74D-BCB2-C2711F71F9EE}">
+  <dimension ref="B2:G22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="2" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B5" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B6" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B7" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="G7" s="13" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B11" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="14"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B12" s="14"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="14"/>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B13" s="14"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="14"/>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B17" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="C17" s="14"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="14"/>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B18" s="14"/>
+      <c r="C18" s="14"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="14"/>
+      <c r="G18" s="14"/>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B19" s="14"/>
+      <c r="C19" s="14"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="14"/>
+      <c r="G19" s="14"/>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B21" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="C21" s="14"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="14"/>
+      <c r="G21" s="14"/>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B22" s="14"/>
+      <c r="C22" s="14"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="14"/>
+      <c r="G22" s="14"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="B11:G13"/>
+    <mergeCell ref="B17:G19"/>
+    <mergeCell ref="B21:G22"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add excel con preguntas
</commit_message>
<xml_diff>
--- a/Graficas.xlsx
+++ b/Graficas.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/katherinegarcia/Documents/Semestre7/SisOps/EjerciciosP2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andreareyes/Desktop/Sistemas Operativos/proyecto2/Paralelismo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EB2B4C6-007E-5B4A-8384-C8209C08177C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73A1D1A3-E130-9443-AECA-2FC477D2B766}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="5" xr2:uid="{842B33A2-C5BF-E74C-A756-B85769930930}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="13900" activeTab="4" xr2:uid="{842B33A2-C5BF-E74C-A756-B85769930930}"/>
   </bookViews>
   <sheets>
     <sheet name="G1" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,6 @@
     <sheet name="G3" sheetId="3" r:id="rId3"/>
     <sheet name="G4" sheetId="4" r:id="rId4"/>
     <sheet name="TODAS" sheetId="5" r:id="rId5"/>
-    <sheet name="Preguntas" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="19">
   <si>
     <t>2 THREADS</t>
   </si>
@@ -97,33 +96,6 @@
   </si>
   <si>
     <t>PROM SECUENCIAL</t>
-  </si>
-  <si>
-    <t>1. ¿Cuál es el modelo de paralelismo más rápido en los 6 escenarios?</t>
-  </si>
-  <si>
-    <t>Los modelos de paralelización mas rápidos son:</t>
-  </si>
-  <si>
-    <t>Archivos</t>
-  </si>
-  <si>
-    <t>Funciones</t>
-  </si>
-  <si>
-    <t>2. ¿Cuál opción modelo de paralelismo tomaría usted y por qué?</t>
-  </si>
-  <si>
-    <t>Depende de los recursos que tengamos y objetivo que el proyecto tenga. En este caso, el modelo más consistente fue la paralelización por archivos. A pesar de las restricciones que se tenían.</t>
-  </si>
-  <si>
-    <t>3. ¿Recomendaría paralelizar tanto archivos y funciones al mismo tiempo?</t>
-  </si>
-  <si>
-    <t>En este caso, el modelo de paralelizacion por funciones y archivos, es el caso mas tardado. Por lo que no lo recomendariamos debido a la limitacion de recursos que se posee.</t>
-  </si>
-  <si>
-    <t>4. Cuál es el factor de mejora de pasar de 1 Core a 2 Core para el proceso que paraleliza los archivos</t>
   </si>
 </sst>
 </file>
@@ -269,7 +241,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -297,10 +269,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -321,7 +289,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="es-MX"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -383,7 +351,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-GT"/>
+          <a:endParaRPr lang="es-GT"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -534,7 +502,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-GT"/>
+            <a:endParaRPr lang="es-GT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="939948160"/>
@@ -593,7 +561,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-GT"/>
+            <a:endParaRPr lang="es-GT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="939946512"/>
@@ -641,7 +609,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-GT"/>
+      <a:endParaRPr lang="es-GT"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -655,7 +623,7 @@
 <file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="es-MX"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -717,7 +685,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-GT"/>
+          <a:endParaRPr lang="es-GT"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1176,7 +1144,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-GT"/>
+            <a:endParaRPr lang="es-GT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="527129392"/>
@@ -1258,7 +1226,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-GT"/>
+              <a:endParaRPr lang="es-GT"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1290,7 +1258,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-GT"/>
+            <a:endParaRPr lang="es-GT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="527127744"/>
@@ -1332,7 +1300,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-GT"/>
+          <a:endParaRPr lang="es-GT"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1369,666 +1337,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-GT"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>PROMEDIO TOTAL DE CADA ESCENARIO</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-GT"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>TODAS!$B$5</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>PROM ARCHIVOS  </c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:multiLvlStrRef>
-              <c:f>TODAS!$C$2:$H$3</c:f>
-              <c:multiLvlStrCache>
-                <c:ptCount val="6"/>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>1 THREAD</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>4 THREADS</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>2 THREADS</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>4 THREADS</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>8 THREADS</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v>8 THREADS</c:v>
-                  </c:pt>
-                </c:lvl>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>1 CORE</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>2 CORES</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v>4 CORES</c:v>
-                  </c:pt>
-                </c:lvl>
-              </c:multiLvlStrCache>
-            </c:multiLvlStrRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>TODAS!$C$5:$H$5</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>9.683720000000001</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>50.752469999999995</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>16.769690000000001</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>20.26613</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>18.319382000000001</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>19.639316999999998</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-9B5F-0B4E-9E52-4F27AE6DCB21}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>TODAS!$B$6</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>PROM FUNCIONES</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:multiLvlStrRef>
-              <c:f>TODAS!$C$2:$H$3</c:f>
-              <c:multiLvlStrCache>
-                <c:ptCount val="6"/>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>1 THREAD</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>4 THREADS</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>2 THREADS</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>4 THREADS</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>8 THREADS</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v>8 THREADS</c:v>
-                  </c:pt>
-                </c:lvl>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>1 CORE</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>2 CORES</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v>4 CORES</c:v>
-                  </c:pt>
-                </c:lvl>
-              </c:multiLvlStrCache>
-            </c:multiLvlStrRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>TODAS!$C$6:$H$6</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>42.643739999999994</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>30.639780000000002</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>26.576080000000001</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>30.234349999999999</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>29.809720000000006</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>13.24981</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-9B5F-0B4E-9E52-4F27AE6DCB21}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>TODAS!$B$7</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>PROM ARCHIVOS Y FUNCIONES</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent4"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:multiLvlStrRef>
-              <c:f>TODAS!$C$2:$H$3</c:f>
-              <c:multiLvlStrCache>
-                <c:ptCount val="6"/>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>1 THREAD</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>4 THREADS</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>2 THREADS</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>4 THREADS</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>8 THREADS</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v>8 THREADS</c:v>
-                  </c:pt>
-                </c:lvl>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>1 CORE</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>2 CORES</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v>4 CORES</c:v>
-                  </c:pt>
-                </c:lvl>
-              </c:multiLvlStrCache>
-            </c:multiLvlStrRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>TODAS!$C$7:$H$7</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>42.149899999999995</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>56.745457999999999</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>24.642440000000001</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>28.830159999999999</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>38.51455</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>18.867979999999999</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-9B5F-0B4E-9E52-4F27AE6DCB21}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:smooth val="0"/>
-        <c:axId val="527127744"/>
-        <c:axId val="527129392"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="527127744"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:title>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-GT"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-GT"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="527129392"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="527129392"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>PROMEDIO EN SEGUNDOS</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-GT"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-GT"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="527127744"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-GT"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-GT"/>
+      <a:endParaRPr lang="es-GT"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2042,7 +1351,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="es-MX"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2109,7 +1418,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-GT"/>
+          <a:endParaRPr lang="es-GT"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -2260,7 +1569,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-GT"/>
+            <a:endParaRPr lang="es-GT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="940016368"/>
@@ -2319,7 +1628,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-GT"/>
+            <a:endParaRPr lang="es-GT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="940014720"/>
@@ -2367,7 +1676,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-GT"/>
+      <a:endParaRPr lang="es-GT"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2381,7 +1690,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="es-MX"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2443,7 +1752,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-GT"/>
+          <a:endParaRPr lang="es-GT"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -2594,7 +1903,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-GT"/>
+            <a:endParaRPr lang="es-GT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1177136239"/>
@@ -2653,7 +1962,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-GT"/>
+            <a:endParaRPr lang="es-GT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1176840175"/>
@@ -2701,7 +2010,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-GT"/>
+      <a:endParaRPr lang="es-GT"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2715,7 +2024,7 @@
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="es-MX"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2777,7 +2086,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-GT"/>
+          <a:endParaRPr lang="es-GT"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -2928,7 +2237,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-GT"/>
+            <a:endParaRPr lang="es-GT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="526917456"/>
@@ -2987,7 +2296,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-GT"/>
+            <a:endParaRPr lang="es-GT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="526915808"/>
@@ -3035,7 +2344,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-GT"/>
+      <a:endParaRPr lang="es-GT"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -3049,7 +2358,7 @@
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="es-MX"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -3111,7 +2420,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-GT"/>
+          <a:endParaRPr lang="es-GT"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -3262,7 +2571,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-GT"/>
+            <a:endParaRPr lang="es-GT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1177136239"/>
@@ -3321,7 +2630,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-GT"/>
+            <a:endParaRPr lang="es-GT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1176840175"/>
@@ -3369,7 +2678,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-GT"/>
+      <a:endParaRPr lang="es-GT"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -3383,7 +2692,7 @@
 <file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="es-MX"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -3445,7 +2754,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-GT"/>
+          <a:endParaRPr lang="es-GT"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -3596,7 +2905,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-GT"/>
+            <a:endParaRPr lang="es-GT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="526917456"/>
@@ -3655,7 +2964,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-GT"/>
+            <a:endParaRPr lang="es-GT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="526915808"/>
@@ -3703,7 +3012,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-GT"/>
+      <a:endParaRPr lang="es-GT"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -3717,7 +3026,7 @@
 <file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="es-MX"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -3779,7 +3088,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-GT"/>
+          <a:endParaRPr lang="es-GT"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -3930,7 +3239,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-GT"/>
+            <a:endParaRPr lang="es-GT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1177136239"/>
@@ -3989,7 +3298,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-GT"/>
+            <a:endParaRPr lang="es-GT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1176840175"/>
@@ -4037,7 +3346,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-GT"/>
+      <a:endParaRPr lang="es-GT"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -4051,7 +3360,7 @@
 <file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="es-MX"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -4332,7 +3641,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-GT"/>
+            <a:endParaRPr lang="es-GT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="526917456"/>
@@ -4391,7 +3700,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-GT"/>
+            <a:endParaRPr lang="es-GT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="526915808"/>
@@ -4411,7 +3720,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-GT"/>
+      <a:endParaRPr lang="es-GT"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -4425,7 +3734,7 @@
 <file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="es-MX"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -4487,7 +3796,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-GT"/>
+          <a:endParaRPr lang="es-GT"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -4647,7 +3956,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-GT"/>
+            <a:endParaRPr lang="es-GT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="526917456"/>
@@ -4703,7 +4012,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-GT"/>
+            <a:endParaRPr lang="es-GT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="526915808"/>
@@ -4751,7 +4060,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-GT"/>
+      <a:endParaRPr lang="es-GT"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -4763,46 +4072,6 @@
 </file>
 
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
-<file path=xl/charts/colors10.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -5163,522 +4432,6 @@
 </file>
 
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
-<file path=xl/charts/style10.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -10717,51 +9470,8 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>50800</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>25400</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>63500</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2BAC841C-25B5-3941-BE83-8CF8F850A4DF}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks/>
-        </xdr:cNvGraphicFramePr>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -12354,7 +11064,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FC59D95-BFDA-464E-9EC5-045460106246}">
   <dimension ref="B2:H7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
@@ -12494,171 +11204,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93C50910-1F7A-B74D-BCB2-C2711F71F9EE}">
-  <dimension ref="B2:G22"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B5" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="12"/>
-      <c r="D5" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B6" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="G6" s="5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B7" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="D7" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="E7" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="F7" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="G7" s="13" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B9" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B11" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="C11" s="14"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="14"/>
-    </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B12" s="14"/>
-      <c r="C12" s="14"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="14"/>
-    </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B13" s="14"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14"/>
-    </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B15" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B17" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="C17" s="14"/>
-      <c r="D17" s="14"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="14"/>
-      <c r="G17" s="14"/>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B18" s="14"/>
-      <c r="C18" s="14"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="14"/>
-      <c r="G18" s="14"/>
-    </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B19" s="14"/>
-      <c r="C19" s="14"/>
-      <c r="D19" s="14"/>
-      <c r="E19" s="14"/>
-      <c r="F19" s="14"/>
-      <c r="G19" s="14"/>
-    </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B21" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="C21" s="14"/>
-      <c r="D21" s="14"/>
-      <c r="E21" s="14"/>
-      <c r="F21" s="14"/>
-      <c r="G21" s="14"/>
-    </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B22" s="14"/>
-      <c r="C22" s="14"/>
-      <c r="D22" s="14"/>
-      <c r="E22" s="14"/>
-      <c r="F22" s="14"/>
-      <c r="G22" s="14"/>
-    </row>
-  </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="D5:F5"/>
-    <mergeCell ref="B11:G13"/>
-    <mergeCell ref="B17:G19"/>
-    <mergeCell ref="B21:G22"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>